<commit_message>
MOS-21370 Updated Feature Road Map
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Processes_Consolidated List_External.xlsx
+++ b/docs/requirements/MOSIP_Processes_Consolidated List_External.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7632B1-F15B-4283-BF0A-EBC3E7AE1684}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB9230A-0CCE-49AF-9D31-ABCEBAAAA2FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Registration" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="92">
   <si>
     <r>
       <t xml:space="preserve">Processes: </t>
@@ -147,9 +147,6 @@
     <t>Impact if Updated</t>
   </si>
   <si>
-    <t>Stage Name</t>
-  </si>
-  <si>
     <t>Packet Receiver Stage</t>
   </si>
   <si>
@@ -345,6 +342,48 @@
   <si>
     <t>If ON - Lost UIN feature will be available on the registration client.
 If OFF - will not be available.</t>
+  </si>
+  <si>
+    <t>Validate Schema of ID Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Files is Present in Packet as per Meta Info </t>
+  </si>
+  <si>
+    <t>Validate Check Sum of the Decrypted Packet</t>
+  </si>
+  <si>
+    <t>Validate Applicant Documents</t>
+  </si>
+  <si>
+    <t>Validate Master Data in ID Obejct</t>
+  </si>
+  <si>
+    <t>Stage Name/Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate if Packet was Created on a Holiday during Packet Creation DateTime </t>
+  </si>
+  <si>
+    <t>Configurable using Config Server Properties</t>
+  </si>
+  <si>
+    <t>Impacts ID JSON validation</t>
+  </si>
+  <si>
+    <t>Impacts ID File validation</t>
+  </si>
+  <si>
+    <t>Impacts Check Sum Validation</t>
+  </si>
+  <si>
+    <t>Impacts Document Validation</t>
+  </si>
+  <si>
+    <t>Impacts Master Data Validation</t>
+  </si>
+  <si>
+    <t>Impacts Timestamp Validation</t>
   </si>
 </sst>
 </file>
@@ -629,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -751,6 +790,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,16 +811,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1690,7 +1732,7 @@
   <autoFilter ref="A2:F26" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="S.No" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Stage Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Stage Name/Process" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Default" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Mindtree Comments" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{B1F48FDA-B6DD-46D5-8D35-13386C811A31}" name="Customer Comments" dataDxfId="1"/>
@@ -1970,28 +2012,28 @@
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="2" customWidth="1"/>
     <col min="2" max="2" width="72" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="23" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="24.6328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.08984375" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -2011,7 +2053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="9" customFormat="1" ht="303.60000000000002" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" s="9" customFormat="1" ht="286" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -2026,7 +2068,7 @@
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2057,7 +2099,7 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row r="4" spans="1:34" s="9" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -2072,7 +2114,7 @@
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2103,7 +2145,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row r="5" spans="1:34" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" s="9" customFormat="1" ht="117" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -2131,7 +2173,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:34" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" s="9" customFormat="1" ht="117" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -2159,7 +2201,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
@@ -2195,7 +2237,7 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
     </row>
-    <row r="8" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
@@ -2231,7 +2273,7 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
     </row>
-    <row r="9" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="5"/>
@@ -2267,7 +2309,7 @@
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
     </row>
-    <row r="10" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="5"/>
@@ -2303,7 +2345,7 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
     </row>
-    <row r="11" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
@@ -2339,7 +2381,7 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
     </row>
-    <row r="12" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
@@ -2375,7 +2417,7 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
     </row>
-    <row r="13" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
@@ -2411,7 +2453,7 @@
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
     </row>
-    <row r="14" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
@@ -2447,7 +2489,7 @@
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
     </row>
-    <row r="15" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
@@ -2483,7 +2525,7 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
     </row>
-    <row r="16" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
@@ -2519,7 +2561,7 @@
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
     </row>
-    <row r="17" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="14"/>
       <c r="C17" s="5"/>
@@ -2555,7 +2597,7 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
     </row>
-    <row r="18" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="20"/>
@@ -2591,7 +2633,7 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
     </row>
-    <row r="19" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
@@ -2627,7 +2669,7 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
-    <row r="20" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -2663,7 +2705,7 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
-    <row r="21" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
@@ -2699,7 +2741,7 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
-    <row r="22" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
@@ -2735,7 +2777,7 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
@@ -2743,7 +2785,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
@@ -2751,7 +2793,7 @@
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -2759,7 +2801,7 @@
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -2783,33 +2825,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DA6495-3DA6-4018-8E4B-7EB4103657AD}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="23" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -2823,13 +2865,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="9" customFormat="1" ht="117" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -2843,10 +2885,10 @@
         <v>23</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -2861,7 +2903,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="9" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="9" customFormat="1" ht="117" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -2875,10 +2917,10 @@
         <v>24</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2893,12 +2935,12 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="9" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="9" customFormat="1" ht="156" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -2908,7 +2950,7 @@
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -2923,12 +2965,12 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="65" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
@@ -2937,10 +2979,10 @@
         <v>22</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -2955,12 +2997,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="65" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>6</v>
@@ -2969,10 +3011,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -2987,12 +3029,12 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="9" customFormat="1" ht="65" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -3001,10 +3043,10 @@
         <v>22</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -3019,12 +3061,12 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="9" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="9" customFormat="1" ht="91" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -3033,10 +3075,10 @@
         <v>22</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3051,21 +3093,21 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28">
         <v>8</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="1"/>
@@ -3081,12 +3123,12 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="39" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>6</v>
@@ -3096,33 +3138,33 @@
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="28">
         <v>10</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="104" x14ac:dyDescent="0.35">
       <c r="A13" s="34">
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>6</v>
@@ -3132,59 +3174,59 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="39" x14ac:dyDescent="0.35">
       <c r="A14" s="34">
         <v>12</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="91" x14ac:dyDescent="0.35">
       <c r="A15" s="34">
         <v>13</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="44">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="39" x14ac:dyDescent="0.35">
+      <c r="A16" s="41">
         <v>14</v>
       </c>
-      <c r="B16" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="46" t="s">
+      <c r="B16" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="47"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="47" t="s">
-        <v>78</v>
+      <c r="F16" s="44" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3203,40 +3245,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="29.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="2"/>
+    <col min="2" max="2" width="29.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6328125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -3251,22 +3293,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>40</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3281,22 +3323,22 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3311,22 +3353,22 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3341,22 +3383,22 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -3371,22 +3413,22 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="21"/>
       <c r="F7" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -3401,22 +3443,22 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -3431,22 +3473,22 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3461,22 +3503,22 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -3491,22 +3533,22 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -3521,22 +3563,22 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -3551,22 +3593,22 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -3581,22 +3623,22 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="9" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>12</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -3611,13 +3653,23 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="21"/>
+    <row r="15" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -3631,13 +3683,23 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="21"/>
+    <row r="16" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -3651,13 +3713,23 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="21"/>
+    <row r="17" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -3671,13 +3743,23 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
+    <row r="18" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="21" t="s">
+        <v>89</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -3691,13 +3773,23 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="21"/>
+    <row r="19" spans="1:18" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -3711,13 +3803,23 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="21"/>
+    <row r="20" spans="1:18" s="9" customFormat="1" ht="39" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
+        <v>18</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="21" t="s">
+        <v>91</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -3731,7 +3833,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
@@ -3751,7 +3853,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
@@ -3771,7 +3873,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
@@ -3779,7 +3881,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
@@ -3787,7 +3889,7 @@
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -3795,7 +3897,7 @@
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -3808,7 +3910,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -3823,27 +3925,27 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="76.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" style="8" customWidth="1"/>
-    <col min="4" max="6" width="24.109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="29.5546875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="6.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="76.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="41.453125" style="8" customWidth="1"/>
+    <col min="4" max="6" width="24.08984375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="29.54296875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -3863,7 +3965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3877,7 +3979,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -3891,7 +3993,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -3905,7 +4007,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:18" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -3931,7 +4033,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -3945,7 +4047,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -3959,7 +4061,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -3973,7 +4075,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -3987,7 +4089,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17"/>
@@ -3995,7 +4097,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="18"/>
@@ -4014,6 +4116,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4220,15 +4331,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4256,6 +4358,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3174CE2-5708-4158-93D0-CBBFFB333158}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E8A634F-74FC-499D-ABEA-0CA6D30F983F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4270,14 +4380,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3174CE2-5708-4158-93D0-CBBFFB333158}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>